<commit_message>
📋 Daily commented tasks report - 2025-07-31
</commit_message>
<xml_diff>
--- a/daily_commented_tasks_2025-07-31.xlsx
+++ b/daily_commented_tasks_2025-07-31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,12 +486,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Riddhi - TIR Prod SAP Auto Export Status</t>
+          <t>Deep</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vrushali-gohel, RiddhiBaraiya</t>
+          <t>ShahDeep5113</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -501,50 +501,10 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Vrushali-gohel</t>
+          <t>ShahDeep5113</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>&lt;img width="1366" height="768" alt="Image" src="https://github.com/user-attachments/assets/25dd218c-6e8a-4b4c-8338-7b1dd88356f3" /&gt;</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2025-07-30</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Issue</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Deep</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ShahDeep5113</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>ShahDeep5113</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
         <is>
           <t xml:space="preserve">1. Works on IPCL Report (Shell Breakage Report) In Database.
 2. Create SPs for this report and updating templates.
@@ -552,6 +512,46 @@
 4. testing Done for Shell Breakage </t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HONDA : TR : SR94291  For  YES/No and Date Validate</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>&lt;img width="903" height="587" alt="Image" src="https://github.com/user-attachments/assets/d1a6e77f-8d7a-4aad-838f-0aae1df7028c" /&gt;</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>2025-07-30</t>
@@ -569,27 +569,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HONDA : TR : SR94291  For  YES/No and Date Validate</t>
+          <t>HONDA : TR :- Batch/Employee Option</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>ShahDeep5113, Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Vishal-Bhaliya</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Vishal-Bhaliya</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>&lt;img width="903" height="587" alt="Image" src="https://github.com/user-attachments/assets/d1a6e77f-8d7a-4aad-838f-0aae1df7028c" /&gt;</t>
+          <t>&lt;img width="903" height="587" alt="Image" src="https://github.com/user-attachments/assets/863c314e-4191-4561-9c97-c0a6995e11a5" /&gt;</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -609,27 +609,28 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HONDA : TR :- Batch/Employee Option</t>
+          <t>NP1141-INC-450913-add edit rights in SCR database for DTC team</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ShahDeep5113, Vishal-Bhaliya</t>
+          <t>Nandini-RI</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>open</t>
+          <t>closed</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Vishal-Bhaliya</t>
+          <t>Nandini-RI</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>&lt;img width="903" height="587" alt="Image" src="https://github.com/user-attachments/assets/863c314e-4191-4561-9c97-c0a6995e11a5" /&gt;</t>
+          <t>Assign all three people to "Editor" role.
+Asked to user for verify.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -649,28 +650,27 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NP1141-INC-450913-add edit rights in SCR database for DTC team</t>
+          <t>Kontoor: Sarge - Re: SARGE ISSUE</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Nandini-RI</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>closed</t>
+          <t>open</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Nandini-RI</t>
+          <t>Vrushali-gohel</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Assign all three people to "Editor" role.
-Asked to user for verify.</t>
+          <t>- Reset user account&lt;M.Elghobary@lotusgarments.com&gt; password in sarge production</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -690,12 +690,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Kontoor: Sarge - Re: SARGE ISSUE</t>
+          <t>Kontoor: SCR0217 - InfoCenter CoC: Edit function amendment []</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Kinjal-Makwana, Ravi-Morichauhan</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>- Reset user account&lt;M.Elghobary@lotusgarments.com&gt; password in sarge production</t>
+          <t>- Apply logic to edit maker data and test.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -730,12 +730,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Kontoor: SCR0217 - InfoCenter CoC: Edit function amendment []</t>
+          <t>Vrushali</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Kinjal-Makwana, Ravi-Morichauhan</t>
+          <t>Vrushali-gohel</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -750,7 +750,9 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>- Apply logic to edit maker data and test.</t>
+          <t xml:space="preserve">- https://github.com/RI-BVN/RamansheeRepo/issues/230 -- Checked log
+- https://github.com/RI-BVN/RamansheeRepo/issues/633 -- reset account password
+- https://github.com/RI-BVN/RamansheeRepo/issues/450 </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -770,12 +772,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Vrushali</t>
+          <t>Miloni</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Vrushali-gohel</t>
+          <t>Miloni-Mehta04</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -785,14 +787,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Vrushali-gohel</t>
+          <t>Miloni-Mehta04</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">- https://github.com/RI-BVN/RamansheeRepo/issues/230 -- Checked log
-- https://github.com/RI-BVN/RamansheeRepo/issues/633 -- reset account password
-- https://github.com/RI-BVN/RamansheeRepo/issues/450 </t>
+          <t>Working on UI for VMI CRS Account Function and some modification in it</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -812,12 +812,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Miloni</t>
+          <t>Ravi</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Miloni-Mehta04</t>
+          <t>Ravi-Morichauhan</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -827,12 +827,14 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Miloni-Mehta04</t>
+          <t>Ravi-Morichauhan</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Working on UI for VMI CRS Account Function and some modification in it</t>
+          <t>1. RoofTopLight Company Stock List – Ensure proper filtering, pagination, and design.
+2. RoofTopLight ConfirmOrder - proper filtering, pagination, and design.
+3. RoofTopLight Challan List - proper fil</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -852,12 +854,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ravi</t>
+          <t>Utsav</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Ravi-Morichauhan</t>
+          <t>Utsav-Patel9</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -867,52 +869,10 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Ravi-Morichauhan</t>
+          <t>Utsav-Patel9</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
-        <is>
-          <t>1. RoofTopLight Company Stock List – Ensure proper filtering, pagination, and design.
-2. RoofTopLight ConfirmOrder - proper filtering, pagination, and design.
-3. RoofTopLight Challan List - proper fil</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2025-07-30</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Issue</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Utsav</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Utsav-Patel9</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Utsav-Patel9</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
         <is>
           <t>Powerapp :
 1. Daily Stock Adjustment List in second screen in add field
@@ -920,42 +880,42 @@
 3. Daily Stock Adjustment List in click on edit and all screen value bind scre</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>2025-07-30</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Issue</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>Rakesh</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Rakesh-Morichauhan</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Rakesh-Morichauhan</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t xml:space="preserve"> 
 1. Add/Update (Alert Massage in Insert successfully completed Or Update Successfully Completed) 
@@ -963,6 +923,46 @@
 3. Department Head List page and Edit models</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>HONDA : SR101180 :Travel billing module</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ShahDeep5113, Vishal-Bhaliya, Urmi-Parmar</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>&lt;img width="800" height="458" alt="Image" src="https://github.com/user-attachments/assets/16cf95b2-3d43-4377-8cf6-0d67a4c3fb0f" /&gt;</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
           <t>2025-07-30</t>
@@ -980,12 +980,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HONDA : SR101180 :Travel billing module</t>
+          <t>Kinjal</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ShahDeep5113, Vishal-Bhaliya, Urmi-Parmar</t>
+          <t>Kinjal-Makwana</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -995,50 +995,10 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Vishal-Bhaliya</t>
+          <t>Kinjal-Makwana</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
-        <is>
-          <t>&lt;img width="800" height="458" alt="Image" src="https://github.com/user-attachments/assets/16cf95b2-3d43-4377-8cf6-0d67a4c3fb0f" /&gt;</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2025-07-30</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Issue</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Kinjal</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Kinjal-Makwana</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Kinjal-Makwana</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
         <is>
           <t>**In 1st Half**
 - Ticket, Outstanding file update
@@ -1047,12 +1007,213 @@
 - #618 - Replied user
 - Weekly meeting from 1 to 2
 **In 2nd Half**
-- #630 - Work and replied user</t>
+- #630 - Work and replied user
+- https</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Riddhi - TIR Prod SAP Auto Export Status</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Vrushali-gohel, RiddhiBaraiya</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Vrushali-gohel</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>&lt;img width="1218" height="560" alt="Image" src="https://github.com/user-attachments/assets/daedf98b-d8ac-4c6e-984f-f702cd561b79" /&gt;</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>HONDA : SR102099 -Emp.Code-12782-Rellocation click forgated</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>&lt;img width="900" height="757" alt="Image" src="https://github.com/user-attachments/assets/2afa467f-943d-45a1-97ad-87fc1694243b" /&gt;</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>HONDA : PR dashboard access - SR99647</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Urmi-Parmar</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>change log shared with  &lt;img width="800" height="458" alt="Image" src="https://github.com/user-attachments/assets/7a420465-48f4-4980-838e-4da8ed0cd776" /&gt;</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>HONDA : SR100081 : Roaster Extra Seat add For Div  based on OP seat margin</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ShahDeep5113, Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Need To correct Some Functionality after discussion with satyaveer san aS ON 30-07-205</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>HONDA : SR104589 - SHE Documents on Employee portal</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Vishal-Bhaliya</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Go live on 30-07-2025 3:30 PM </t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
         </is>
       </c>
     </row>

</xml_diff>